<commit_message>
update scrape code & DEC 2020 scrape
</commit_message>
<xml_diff>
--- a/FTSE_350_FIRM_LIST.xlsx
+++ b/FTSE_350_FIRM_LIST.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ms3453n\OneDrive - University of Greenwich\GitHub\FTSE_350_LIST\"/>
     </mc:Choice>
@@ -16,6 +16,7 @@
     <sheet name="2018-11" sheetId="1" r:id="rId1"/>
     <sheet name="2019-08-16" sheetId="2" r:id="rId2"/>
     <sheet name="2020-01-09" sheetId="3" r:id="rId3"/>
+    <sheet name="2020-12-22" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5103" uniqueCount="2201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5807" uniqueCount="2346">
   <si>
     <t>CODE</t>
   </si>
@@ -6633,6 +6634,441 @@
   </si>
   <si>
     <t>twitter_search_name</t>
+  </si>
+  <si>
+    <t>.x..i..</t>
+  </si>
+  <si>
+    <t>329</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>331</t>
+  </si>
+  <si>
+    <t>332</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>334</t>
+  </si>
+  <si>
+    <t>335</t>
+  </si>
+  <si>
+    <t>336</t>
+  </si>
+  <si>
+    <t>337</t>
+  </si>
+  <si>
+    <t>338</t>
+  </si>
+  <si>
+    <t>339</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>341</t>
+  </si>
+  <si>
+    <t>342</t>
+  </si>
+  <si>
+    <t>343</t>
+  </si>
+  <si>
+    <t>344</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>346</t>
+  </si>
+  <si>
+    <t>347</t>
+  </si>
+  <si>
+    <t>348</t>
+  </si>
+  <si>
+    <t>349</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
+    <t>351</t>
+  </si>
+  <si>
+    <t>3.22</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>2.25</t>
+  </si>
+  <si>
+    <t>4.45</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>10.6</t>
+  </si>
+  <si>
+    <t>4.05</t>
+  </si>
+  <si>
+    <t>1.56</t>
+  </si>
+  <si>
+    <t>10.8</t>
+  </si>
+  <si>
+    <t>31.5</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>32.5</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>27.5</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>29.2</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>2.45</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>13.5</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>14.5</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>1.65</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.30</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>0.20</t>
+  </si>
+  <si>
+    <t>4.00</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>-0.20</t>
+  </si>
+  <si>
+    <t>-0.10</t>
+  </si>
+  <si>
+    <t>-0.50</t>
+  </si>
+  <si>
+    <t>-0.5</t>
+  </si>
+  <si>
+    <t>-0.2</t>
+  </si>
+  <si>
+    <t>-1.5</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>-8</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>-1.4</t>
+  </si>
+  <si>
+    <t>-0.3</t>
+  </si>
+  <si>
+    <t>-6</t>
+  </si>
+  <si>
+    <t>-3.5</t>
+  </si>
+  <si>
+    <t>-0.6</t>
+  </si>
+  <si>
+    <t>-7</t>
+  </si>
+  <si>
+    <t>-5</t>
+  </si>
+  <si>
+    <t>-0.8</t>
+  </si>
+  <si>
+    <t>-50</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>-2.5</t>
+  </si>
+  <si>
+    <t>-9.5</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-3.8</t>
+  </si>
+  <si>
+    <t>-10</t>
+  </si>
+  <si>
+    <t>-1.7</t>
+  </si>
+  <si>
+    <t>-2.2</t>
+  </si>
+  <si>
+    <t>-2.3</t>
+  </si>
+  <si>
+    <t>-8.5</t>
+  </si>
+  <si>
+    <t>-15</t>
+  </si>
+  <si>
+    <t>-6.2</t>
+  </si>
+  <si>
+    <t>-0.7</t>
+  </si>
+  <si>
+    <t>-7.5</t>
+  </si>
+  <si>
+    <t>-0.25</t>
+  </si>
+  <si>
+    <t>-72</t>
+  </si>
+  <si>
+    <t>-0.9</t>
+  </si>
+  <si>
+    <t>-4.6</t>
+  </si>
+  <si>
+    <t>-1.2</t>
+  </si>
+  <si>
+    <t>-25</t>
+  </si>
+  <si>
+    <t>-1.1</t>
+  </si>
+  <si>
+    <t>-85</t>
+  </si>
+  <si>
+    <t>-9</t>
+  </si>
+  <si>
+    <t>-17</t>
+  </si>
+  <si>
+    <t>-47</t>
+  </si>
+  <si>
+    <t>-11</t>
   </si>
 </sst>
 </file>
@@ -7119,11 +7555,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -7487,7 +7925,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -14545,7 +14983,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -22659,7 +23097,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="55.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -34177,4 +34615,3887 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>2201</v>
+      </c>
+      <c r="C1" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2225</v>
+      </c>
+      <c r="C2" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2226</v>
+      </c>
+      <c r="C3" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C4" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C5" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2227</v>
+      </c>
+      <c r="C6" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C7" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C8" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C9" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C10" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2228</v>
+      </c>
+      <c r="C11" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2229</v>
+      </c>
+      <c r="C12" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C13" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C14" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2230</v>
+      </c>
+      <c r="C15" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C16" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C17" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2231</v>
+      </c>
+      <c r="C18" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2232</v>
+      </c>
+      <c r="C19" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2233</v>
+      </c>
+      <c r="C20" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2234</v>
+      </c>
+      <c r="C21" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2235</v>
+      </c>
+      <c r="C22" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C23" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C24" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C25" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2236</v>
+      </c>
+      <c r="C26" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2237</v>
+      </c>
+      <c r="C27" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2238</v>
+      </c>
+      <c r="C28" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2239</v>
+      </c>
+      <c r="C29" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2240</v>
+      </c>
+      <c r="C30" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C31" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C32" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2241</v>
+      </c>
+      <c r="C33" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2242</v>
+      </c>
+      <c r="C34" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C35" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C36" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C37" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2243</v>
+      </c>
+      <c r="C38" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C39" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2238</v>
+      </c>
+      <c r="C40" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2244</v>
+      </c>
+      <c r="C41" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C42" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2245</v>
+      </c>
+      <c r="C43" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C44" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C45" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2246</v>
+      </c>
+      <c r="C46" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C47" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C48" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2247</v>
+      </c>
+      <c r="C49" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C50" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2248</v>
+      </c>
+      <c r="C51" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2249</v>
+      </c>
+      <c r="C52" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2250</v>
+      </c>
+      <c r="C53" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2251</v>
+      </c>
+      <c r="C54" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C55" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2249</v>
+      </c>
+      <c r="C56" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C57" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2252</v>
+      </c>
+      <c r="C58" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2253</v>
+      </c>
+      <c r="C59" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C60" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C61" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2254</v>
+      </c>
+      <c r="C62" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2255</v>
+      </c>
+      <c r="C63" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C64" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C65" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2232</v>
+      </c>
+      <c r="C66" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C67" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C68" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C69" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2256</v>
+      </c>
+      <c r="C70" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C71" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C72" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2257</v>
+      </c>
+      <c r="C73" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C74" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2258</v>
+      </c>
+      <c r="C75" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2251</v>
+      </c>
+      <c r="C76" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2251</v>
+      </c>
+      <c r="C77" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2259</v>
+      </c>
+      <c r="C78" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B79" t="s">
+        <v>2260</v>
+      </c>
+      <c r="C79" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C80" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B81" t="s">
+        <v>2261</v>
+      </c>
+      <c r="C81" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B82" t="s">
+        <v>2254</v>
+      </c>
+      <c r="C82" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2250</v>
+      </c>
+      <c r="C83" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C84" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2260</v>
+      </c>
+      <c r="C85" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C86" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C87" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2262</v>
+      </c>
+      <c r="C88" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2231</v>
+      </c>
+      <c r="C89" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C90" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C91" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C92" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2263</v>
+      </c>
+      <c r="C93" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C94" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2264</v>
+      </c>
+      <c r="C95" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C96" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C97" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C98" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C99" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C100" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2265</v>
+      </c>
+      <c r="C101" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C102" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C103" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B104" t="s">
+        <v>2247</v>
+      </c>
+      <c r="C104" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C105" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2249</v>
+      </c>
+      <c r="C106" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C107" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B108" t="s">
+        <v>2266</v>
+      </c>
+      <c r="C108" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C109" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C110" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B111" t="s">
+        <v>2267</v>
+      </c>
+      <c r="C111" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2268</v>
+      </c>
+      <c r="C112" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C113" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C114" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2269</v>
+      </c>
+      <c r="C115" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2270</v>
+      </c>
+      <c r="C116" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B117" t="s">
+        <v>2271</v>
+      </c>
+      <c r="C117" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2272</v>
+      </c>
+      <c r="C118" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C119" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C120" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C121" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B122" t="s">
+        <v>2273</v>
+      </c>
+      <c r="C122" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B123" t="s">
+        <v>2274</v>
+      </c>
+      <c r="C123" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2275</v>
+      </c>
+      <c r="C124" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C125" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C126" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B127" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C127" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2277</v>
+      </c>
+      <c r="C128" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C129" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B130" t="s">
+        <v>2243</v>
+      </c>
+      <c r="C130" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B131" t="s">
+        <v>2266</v>
+      </c>
+      <c r="C131" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B132" t="s">
+        <v>2249</v>
+      </c>
+      <c r="C132" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C133" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B134" t="s">
+        <v>2278</v>
+      </c>
+      <c r="C134" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B135" t="s">
+        <v>2279</v>
+      </c>
+      <c r="C135" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2280</v>
+      </c>
+      <c r="C136" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B137" t="s">
+        <v>2281</v>
+      </c>
+      <c r="C137" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B138" t="s">
+        <v>2281</v>
+      </c>
+      <c r="C138" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C139" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C140" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B141" t="s">
+        <v>2265</v>
+      </c>
+      <c r="C141" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2256</v>
+      </c>
+      <c r="C142" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C143" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C144" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C145" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C146" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C147" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B148" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C148" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B149" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C149" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C150" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C151" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B152" t="s">
+        <v>2275</v>
+      </c>
+      <c r="C152" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C153" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C154" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B155" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C155" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B156" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C156" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C157" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C158" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B159" t="s">
+        <v>2282</v>
+      </c>
+      <c r="C159" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B160" t="s">
+        <v>2283</v>
+      </c>
+      <c r="C160" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C161" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B162" t="s">
+        <v>2272</v>
+      </c>
+      <c r="C162" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C163" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C164" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C165" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C166" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B167" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C167" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B168" t="s">
+        <v>2269</v>
+      </c>
+      <c r="C168" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B169" t="s">
+        <v>2284</v>
+      </c>
+      <c r="C169" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B170" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C170" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B171" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C171" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B172" t="s">
+        <v>2267</v>
+      </c>
+      <c r="C172" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B173" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C173" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B174" t="s">
+        <v>2285</v>
+      </c>
+      <c r="C174" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B175" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C175" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B176" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C176" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B177" t="s">
+        <v>2282</v>
+      </c>
+      <c r="C177" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B178" t="s">
+        <v>2269</v>
+      </c>
+      <c r="C178" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B179" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C179" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B180" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C180" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B181" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C181" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B182" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C182" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B183" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C183" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B184" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C184" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B185" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C185" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B186" t="s">
+        <v>2250</v>
+      </c>
+      <c r="C186" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B187" t="s">
+        <v>2286</v>
+      </c>
+      <c r="C187" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B188" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C188" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B189" t="s">
+        <v>2287</v>
+      </c>
+      <c r="C189" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B190" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C190" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B191" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C191" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B192" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C192" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B193" t="s">
+        <v>2288</v>
+      </c>
+      <c r="C193" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B194" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C194" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B195" t="s">
+        <v>2274</v>
+      </c>
+      <c r="C195" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B196" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C196" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B197" t="s">
+        <v>2289</v>
+      </c>
+      <c r="C197" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B198" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C198" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B199" t="s">
+        <v>2283</v>
+      </c>
+      <c r="C199" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B200" t="s">
+        <v>2290</v>
+      </c>
+      <c r="C200" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B201" t="s">
+        <v>2286</v>
+      </c>
+      <c r="C201" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B202" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C202" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B203" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C203" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B204" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C204" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B205" t="s">
+        <v>2286</v>
+      </c>
+      <c r="C205" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B206" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C206" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B207" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C207" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B208" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C208" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B209" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C209" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B210" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C210" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B211" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C211" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B212" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C212" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B213" t="s">
+        <v>2284</v>
+      </c>
+      <c r="C213" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B214" t="s">
+        <v>2291</v>
+      </c>
+      <c r="C214" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B215" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C215" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B216" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C216" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B217" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C217" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B218" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C218" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B219" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C219" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B220" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C220" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B221" t="s">
+        <v>2250</v>
+      </c>
+      <c r="C221" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B222" t="s">
+        <v>2249</v>
+      </c>
+      <c r="C222" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B223" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C223" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B224" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C224" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B225" t="s">
+        <v>2286</v>
+      </c>
+      <c r="C225" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B226" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C226" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B227" t="s">
+        <v>2293</v>
+      </c>
+      <c r="C227" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B228" t="s">
+        <v>2286</v>
+      </c>
+      <c r="C228" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B229" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C229" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B230" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C230" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B231" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C231" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B232" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C232" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B233" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C233" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B234" t="s">
+        <v>2286</v>
+      </c>
+      <c r="C234" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B235" t="s">
+        <v>2292</v>
+      </c>
+      <c r="C235" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B236" t="s">
+        <v>2294</v>
+      </c>
+      <c r="C236" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B237" t="s">
+        <v>2289</v>
+      </c>
+      <c r="C237" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B238" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C238" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B239" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C239" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B240" t="s">
+        <v>2284</v>
+      </c>
+      <c r="C240" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B241" t="s">
+        <v>2276</v>
+      </c>
+      <c r="C241" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B242" t="s">
+        <v>2295</v>
+      </c>
+      <c r="C242" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B243" t="s">
+        <v>2296</v>
+      </c>
+      <c r="C243" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B244" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C244" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B245" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C245" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B246" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C246" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B247" t="s">
+        <v>2299</v>
+      </c>
+      <c r="C247" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B248" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C248" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B249" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C249" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B250" t="s">
+        <v>2300</v>
+      </c>
+      <c r="C250" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B251" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C251" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B252" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C252" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B253" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C253" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B254" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C254" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B255" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C255" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B256" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C256" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B257" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C257" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B258" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C258" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B259" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C259" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B260" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C260" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B261" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C261" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B262" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C262" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B263" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C263" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B264" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C264" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B265" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C265" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B266" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C266" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B267" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C267" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B268" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C268" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B269" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C269" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B270" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C270" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B271" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C271" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B272" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C272" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B273" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C273" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B274" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C274" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B275" t="s">
+        <v>2301</v>
+      </c>
+      <c r="C275" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B276" t="s">
+        <v>2302</v>
+      </c>
+      <c r="C276" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B277" t="s">
+        <v>2303</v>
+      </c>
+      <c r="C277" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B278" t="s">
+        <v>2302</v>
+      </c>
+      <c r="C278" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B279" t="s">
+        <v>2304</v>
+      </c>
+      <c r="C279" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B280" t="s">
+        <v>2304</v>
+      </c>
+      <c r="C280" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B281" t="s">
+        <v>2302</v>
+      </c>
+      <c r="C281" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B282" t="s">
+        <v>2305</v>
+      </c>
+      <c r="C282" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B283" t="s">
+        <v>2306</v>
+      </c>
+      <c r="C283" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B284" t="s">
+        <v>2307</v>
+      </c>
+      <c r="C284" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B285" t="s">
+        <v>2307</v>
+      </c>
+      <c r="C285" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B286" t="s">
+        <v>2305</v>
+      </c>
+      <c r="C286" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B287" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C287" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B288" t="s">
+        <v>2309</v>
+      </c>
+      <c r="C288" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B289" t="s">
+        <v>2310</v>
+      </c>
+      <c r="C289" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B290" t="s">
+        <v>2311</v>
+      </c>
+      <c r="C290" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B291" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C291" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B292" t="s">
+        <v>2312</v>
+      </c>
+      <c r="C292" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B293" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C293" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B294" t="s">
+        <v>2306</v>
+      </c>
+      <c r="C294" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B295" t="s">
+        <v>2310</v>
+      </c>
+      <c r="C295" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B296" t="s">
+        <v>2305</v>
+      </c>
+      <c r="C296" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B297" t="s">
+        <v>2314</v>
+      </c>
+      <c r="C297" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B298" t="s">
+        <v>2305</v>
+      </c>
+      <c r="C298" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B299" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C299" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B300" t="s">
+        <v>2316</v>
+      </c>
+      <c r="C300" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B301" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C301" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B302" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C302" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B303" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C303" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B304" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C304" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B305" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C305" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B306" t="s">
+        <v>2321</v>
+      </c>
+      <c r="C306" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B307" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C307" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B308" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C308" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B309" t="s">
+        <v>2312</v>
+      </c>
+      <c r="C309" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B310" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C310" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B311" t="s">
+        <v>2324</v>
+      </c>
+      <c r="C311" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B312" t="s">
+        <v>2325</v>
+      </c>
+      <c r="C312" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B313" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C313" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B314" t="s">
+        <v>2326</v>
+      </c>
+      <c r="C314" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B315" t="s">
+        <v>2325</v>
+      </c>
+      <c r="C315" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B316" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C316" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B317" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C317" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B318" t="s">
+        <v>2327</v>
+      </c>
+      <c r="C318" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B319" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C319" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B320" t="s">
+        <v>2309</v>
+      </c>
+      <c r="C320" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B321" t="s">
+        <v>2309</v>
+      </c>
+      <c r="C321" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B322" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C322" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B323" t="s">
+        <v>2329</v>
+      </c>
+      <c r="C323" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B324" t="s">
+        <v>2330</v>
+      </c>
+      <c r="C324" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B325" t="s">
+        <v>2311</v>
+      </c>
+      <c r="C325" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B326" t="s">
+        <v>2307</v>
+      </c>
+      <c r="C326" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B327" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C327" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B328" t="s">
+        <v>2331</v>
+      </c>
+      <c r="C328" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B329" t="s">
+        <v>2327</v>
+      </c>
+      <c r="C329" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s">
+        <v>2202</v>
+      </c>
+      <c r="B330" t="s">
+        <v>2332</v>
+      </c>
+      <c r="C330" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s">
+        <v>2203</v>
+      </c>
+      <c r="B331" t="s">
+        <v>2332</v>
+      </c>
+      <c r="C331" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s">
+        <v>2204</v>
+      </c>
+      <c r="B332" t="s">
+        <v>2333</v>
+      </c>
+      <c r="C332" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s">
+        <v>2205</v>
+      </c>
+      <c r="B333" t="s">
+        <v>2334</v>
+      </c>
+      <c r="C333" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s">
+        <v>2206</v>
+      </c>
+      <c r="B334" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C334" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s">
+        <v>2207</v>
+      </c>
+      <c r="B335" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C335" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B336" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C336" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s">
+        <v>2209</v>
+      </c>
+      <c r="B337" t="s">
+        <v>2335</v>
+      </c>
+      <c r="C337" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B338" t="s">
+        <v>2331</v>
+      </c>
+      <c r="C338" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B339" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C339" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B340" t="s">
+        <v>2337</v>
+      </c>
+      <c r="C340" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B341" t="s">
+        <v>2338</v>
+      </c>
+      <c r="C341" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B342" t="s">
+        <v>2339</v>
+      </c>
+      <c r="C342" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s">
+        <v>2215</v>
+      </c>
+      <c r="B343" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C343" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B344" t="s">
+        <v>2327</v>
+      </c>
+      <c r="C344" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B345" t="s">
+        <v>2341</v>
+      </c>
+      <c r="C345" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B346" t="s">
+        <v>2326</v>
+      </c>
+      <c r="C346" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B347" t="s">
+        <v>2342</v>
+      </c>
+      <c r="C347" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B348" t="s">
+        <v>2343</v>
+      </c>
+      <c r="C348" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B349" t="s">
+        <v>2314</v>
+      </c>
+      <c r="C349" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>2222</v>
+      </c>
+      <c r="B350" t="s">
+        <v>2314</v>
+      </c>
+      <c r="C350" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B351" t="s">
+        <v>2344</v>
+      </c>
+      <c r="C351" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s">
+        <v>2224</v>
+      </c>
+      <c r="B352" t="s">
+        <v>2345</v>
+      </c>
+      <c r="C352" t="n" s="5">
+        <v>44187.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>